<commit_message>
Add and normalize executive board data sheets
</commit_message>
<xml_diff>
--- a/statistics_files/nekls_executive_board/2024/2024_09_next_statistics_for_executive_board.xlsx
+++ b/statistics_files/nekls_executive_board/2024/2024_09_next_statistics_for_executive_board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\nekls_executive_board\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99FEF439-0CBE-4F4F-89B3-DC5ECA5AC422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF5B790-7404-43C1-BF7A-680D666BCC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{173C74C7-6DED-436A-89F4-F7E38458C5AD}"/>
   </bookViews>
@@ -721,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C6C002-615A-4761-A196-B7586E04732E}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>